<commit_message>
MP Taxonomy with River Data
</commit_message>
<xml_diff>
--- a/data/Microplastic_Taxonomy/Microplastics_DataPortal_Clean_Color.xlsx
+++ b/data/Microplastic_Taxonomy/Microplastics_DataPortal_Clean_Color.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahhapich/Desktop/Microplastic_Data_Portal-main/data/Microplastic_Taxonomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E91AE47-71B8-5644-B36D-4CAD07F6EA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999111C1-9324-5A46-9229-EF8E3D714180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="740" windowWidth="10140" windowHeight="11720" xr2:uid="{B90667D5-789B-1443-AC19-B88537148C27}"/>
+    <workbookView xWindow="-29060" yWindow="-4240" windowWidth="10140" windowHeight="11720" xr2:uid="{B90667D5-789B-1443-AC19-B88537148C27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Color</t>
   </si>
@@ -137,6 +137,21 @@
   </si>
   <si>
     <t>10.1016/j.scitotenv.2021.148001</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Grey</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>doi.org/10.1016/j.envpol.2016.01.018</t>
   </si>
 </sst>
 </file>
@@ -488,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50991143-600A-2E43-8D13-7BA9D88AAC24}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,6 +691,27 @@
         <v>16</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>